<commit_message>
Count on J5 in hand-mount BOM list.
</commit_message>
<xml_diff>
--- a/SOURCES/kiCAD/FreeDSP_OCTAVIA_0v2_BOM-LIST.xlsx
+++ b/SOURCES/kiCAD/FreeDSP_OCTAVIA_0v2_BOM-LIST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HILO/Documents/KICAD_DATA/FreeDSP-OCTAVIA/FreeDSP_OCTAVIA/SOURCES/kiCAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A791C855-D3BD-1941-A6DD-0E9A118C8E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10702240-9C43-084D-9EB4-8239B60435D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="2440" windowWidth="41120" windowHeight="21040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="2440" windowWidth="41120" windowHeight="21040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Separate" sheetId="3" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3190" uniqueCount="1146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3190" uniqueCount="1147">
   <si>
     <t>Date:</t>
   </si>
@@ -3562,6 +3562,10 @@
   </si>
   <si>
     <t>25AA1024</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>J16, J17, J20, J21, J5</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4131,7 +4135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I475"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A414" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F432" sqref="F432"/>
     </sheetView>
@@ -17143,9 +17147,9 @@
   </sheetPr>
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -18111,10 +18115,10 @@
         <v>981</v>
       </c>
       <c r="B20" s="26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>982</v>
+        <v>1146</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>83</v>

</xml_diff>

<commit_message>
R7 R33 Value Changed
</commit_message>
<xml_diff>
--- a/SOURCES/kiCAD/FreeDSP_OCTAVIA_0v2_BOM-LIST.xlsx
+++ b/SOURCES/kiCAD/FreeDSP_OCTAVIA_0v2_BOM-LIST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HILO/Documents/KICAD_DATA/FreeDSP-OCTAVIA/FreeDSP_OCTAVIA/SOURCES/kiCAD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10702240-9C43-084D-9EB4-8239B60435D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1E52B3-02BF-F14C-B320-AF8BB3402EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="620" yWindow="2440" windowWidth="41120" windowHeight="21040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8800" yWindow="3420" windowWidth="41120" windowHeight="21040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Separate" sheetId="3" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3190" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3192" uniqueCount="1149">
   <si>
     <t>Date:</t>
   </si>
@@ -3144,9 +3144,6 @@
     <t>84</t>
   </si>
   <si>
-    <t>R7, R33, R42, R65, R93, R96, R98</t>
-  </si>
-  <si>
     <t>85</t>
   </si>
   <si>
@@ -3250,9 +3247,6 @@
   </si>
   <si>
     <t>104</t>
-  </si>
-  <si>
-    <t>R49, R76, R84</t>
   </si>
   <si>
     <t>105</t>
@@ -3566,6 +3560,42 @@
   </si>
   <si>
     <t>J16, J17, J20, J21, J5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3.3k</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>R42, R65, R93, R96, R98</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">R7, R33, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R49, R76, R84</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Changed for expanding Supply Voltage</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3573,7 +3603,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3645,6 +3675,29 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -3729,7 +3782,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3813,6 +3866,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4135,9 +4197,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I475"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A414" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F432" sqref="F432"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A342" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B359" sqref="B359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -4155,7 +4217,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="33">
       <c r="A1" s="9" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -4202,13 +4264,13 @@
         <v>194</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
@@ -4218,10 +4280,10 @@
         <v>5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -4229,7 +4291,7 @@
     <row r="6" spans="1:9">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -4242,7 +4304,7 @@
         <v>74</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -4440,7 +4502,7 @@
     <row r="17" spans="1:9">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
@@ -4459,7 +4521,7 @@
     <row r="18" spans="1:9">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
@@ -4478,7 +4540,7 @@
     <row r="19" spans="1:9">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
@@ -4497,7 +4559,7 @@
     <row r="20" spans="1:9">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5" t="s">
@@ -4512,13 +4574,13 @@
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
@@ -4537,7 +4599,7 @@
     <row r="22" spans="1:9">
       <c r="A22" s="5"/>
       <c r="B22" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5" t="s">
@@ -4550,17 +4612,17 @@
         <v>78</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="5"/>
       <c r="B23" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5" t="s">
@@ -4573,7 +4635,7 @@
         <v>80</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -4581,7 +4643,7 @@
     <row r="24" spans="1:9">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
@@ -4600,7 +4662,7 @@
     <row r="25" spans="1:9">
       <c r="A25" s="5"/>
       <c r="B25" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5" t="s">
@@ -4615,13 +4677,13 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
@@ -4636,13 +4698,13 @@
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="5"/>
       <c r="B27" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
@@ -4657,13 +4719,13 @@
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="5"/>
       <c r="B28" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
@@ -4678,13 +4740,13 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="5"/>
       <c r="B29" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
@@ -4703,7 +4765,7 @@
     <row r="30" spans="1:9">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
@@ -4722,7 +4784,7 @@
     <row r="31" spans="1:9">
       <c r="A31" s="5"/>
       <c r="B31" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
@@ -4741,7 +4803,7 @@
     <row r="32" spans="1:9">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
@@ -4760,7 +4822,7 @@
     <row r="33" spans="1:9">
       <c r="A33" s="5"/>
       <c r="B33" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5" t="s">
@@ -4779,7 +4841,7 @@
     <row r="34" spans="1:9">
       <c r="A34" s="5"/>
       <c r="B34" s="5" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5" t="s">
@@ -5043,7 +5105,7 @@
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -10940,19 +11002,21 @@
     <row r="357" spans="1:9">
       <c r="A357" s="5"/>
       <c r="B357" s="5" t="s">
-        <v>577</v>
+        <v>632</v>
       </c>
       <c r="C357" s="5"/>
       <c r="D357" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="E357" s="5" t="s">
-        <v>116</v>
+      <c r="E357" s="30" t="s">
+        <v>1145</v>
       </c>
       <c r="F357" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G357" s="5"/>
+      <c r="G357" s="30" t="s">
+        <v>1148</v>
+      </c>
       <c r="H357" s="5"/>
       <c r="I357" s="5"/>
     </row>
@@ -10978,19 +11042,21 @@
     <row r="359" spans="1:9">
       <c r="A359" s="5"/>
       <c r="B359" s="5" t="s">
-        <v>577</v>
+        <v>632</v>
       </c>
       <c r="C359" s="5"/>
       <c r="D359" s="5" t="s">
         <v>611</v>
       </c>
-      <c r="E359" s="5" t="s">
-        <v>116</v>
+      <c r="E359" s="30" t="s">
+        <v>1145</v>
       </c>
       <c r="F359" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G359" s="5"/>
+      <c r="G359" s="30" t="s">
+        <v>1148</v>
+      </c>
       <c r="H359" s="5"/>
       <c r="I359" s="5"/>
     </row>
@@ -11238,7 +11304,7 @@
         <v>113</v>
       </c>
       <c r="G372" s="5" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="H372" s="5"/>
       <c r="I372" s="5"/>
@@ -11905,7 +11971,7 @@
         <v>113</v>
       </c>
       <c r="G407" s="5" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="H407" s="5"/>
       <c r="I407" s="5"/>
@@ -11926,7 +11992,7 @@
         <v>113</v>
       </c>
       <c r="G408" s="5" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="H408" s="5"/>
       <c r="I408" s="5"/>
@@ -11947,7 +12013,7 @@
         <v>113</v>
       </c>
       <c r="G409" s="5" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="H409" s="5"/>
       <c r="I409" s="5"/>
@@ -11968,7 +12034,7 @@
         <v>113</v>
       </c>
       <c r="G410" s="5" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="H410" s="5"/>
       <c r="I410" s="5"/>
@@ -12217,7 +12283,7 @@
         <v>18</v>
       </c>
       <c r="G423" s="5" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="H423" s="5"/>
       <c r="I423" s="5"/>
@@ -12232,7 +12298,7 @@
         <v>865</v>
       </c>
       <c r="E424" s="5" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="F424" s="5" t="s">
         <v>168</v>
@@ -12911,7 +12977,7 @@
         <v>170</v>
       </c>
       <c r="G459" s="5" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="H459" s="5"/>
       <c r="I459" s="5"/>
@@ -12932,7 +12998,7 @@
         <v>170</v>
       </c>
       <c r="G460" s="5" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="H460" s="5"/>
       <c r="I460" s="5"/>
@@ -12953,7 +13019,7 @@
         <v>170</v>
       </c>
       <c r="G461" s="5" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="H461" s="5"/>
       <c r="I461" s="5"/>
@@ -12974,7 +13040,7 @@
         <v>170</v>
       </c>
       <c r="G462" s="5" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="H462" s="5"/>
       <c r="I462" s="5"/>
@@ -13264,7 +13330,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76:XFD76"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -13275,7 +13341,7 @@
   <sheetData>
     <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="3" spans="1:29" s="8" customFormat="1" ht="21">
@@ -15695,10 +15761,10 @@
         <v>1019</v>
       </c>
       <c r="B87" s="8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>1020</v>
+        <v>1146</v>
       </c>
       <c r="D87" t="s">
         <v>116</v>
@@ -15718,13 +15784,13 @@
     </row>
     <row r="88" spans="1:19" ht="21">
       <c r="A88" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B88" s="8">
         <v>2</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D88" t="s">
         <v>110</v>
@@ -15744,13 +15810,13 @@
     </row>
     <row r="89" spans="1:19" ht="21">
       <c r="A89" s="1" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B89" s="8">
         <v>2</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D89" t="s">
         <v>30</v>
@@ -15770,7 +15836,7 @@
     </row>
     <row r="90" spans="1:19" ht="21">
       <c r="A90" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B90" s="8">
         <v>1</v>
@@ -15793,7 +15859,7 @@
     </row>
     <row r="91" spans="1:19" ht="21">
       <c r="A91" s="1" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B91" s="8">
         <v>1</v>
@@ -15816,13 +15882,13 @@
     </row>
     <row r="92" spans="1:19" ht="21">
       <c r="A92" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B92" s="8">
         <v>2</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D92" t="s">
         <v>118</v>
@@ -15839,7 +15905,7 @@
     </row>
     <row r="93" spans="1:19" ht="21">
       <c r="A93" s="1" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B93" s="8">
         <v>1</v>
@@ -15862,13 +15928,13 @@
     </row>
     <row r="94" spans="1:19" ht="21">
       <c r="A94" s="1" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B94" s="8">
         <v>3</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D94" t="s">
         <v>112</v>
@@ -15885,13 +15951,13 @@
     </row>
     <row r="95" spans="1:19" ht="21">
       <c r="A95" s="1" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="B95" s="8">
         <v>6</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D95" t="s">
         <v>116</v>
@@ -15908,13 +15974,13 @@
     </row>
     <row r="96" spans="1:19" ht="21">
       <c r="A96" s="1" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B96" s="8">
         <v>2</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D96" t="s">
         <v>120</v>
@@ -15931,13 +15997,13 @@
     </row>
     <row r="97" spans="1:19" ht="21">
       <c r="A97" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B97" s="8">
         <v>2</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D97" t="s">
         <v>121</v>
@@ -15954,13 +16020,13 @@
     </row>
     <row r="98" spans="1:19" ht="21">
       <c r="A98" s="1" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B98" s="8">
         <v>2</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D98" t="s">
         <v>122</v>
@@ -15977,13 +16043,13 @@
     </row>
     <row r="99" spans="1:19" ht="21">
       <c r="A99" s="1" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B99" s="8">
         <v>5</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D99" t="s">
         <v>110</v>
@@ -16000,7 +16066,7 @@
     </row>
     <row r="100" spans="1:19" ht="21">
       <c r="A100" s="1" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="B100" s="8">
         <v>1</v>
@@ -16023,13 +16089,13 @@
     </row>
     <row r="101" spans="1:19" ht="63">
       <c r="A101" s="1" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="B101" s="8">
         <v>25</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D101" t="s">
         <v>124</v>
@@ -16049,13 +16115,13 @@
     </row>
     <row r="102" spans="1:19" ht="21">
       <c r="A102" s="1" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B102" s="8">
         <v>7</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D102" t="s">
         <v>30</v>
@@ -16075,13 +16141,13 @@
     </row>
     <row r="103" spans="1:19" ht="42">
       <c r="A103" s="1" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B103" s="8">
         <v>10</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D103" t="s">
         <v>125</v>
@@ -16101,13 +16167,13 @@
     </row>
     <row r="104" spans="1:19" ht="21">
       <c r="A104" s="1" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B104" s="8">
         <v>5</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D104" t="s">
         <v>126</v>
@@ -16127,13 +16193,13 @@
     </row>
     <row r="105" spans="1:19" ht="21">
       <c r="A105" s="1" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="B105" s="8">
         <v>2</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D105" t="s">
         <v>112</v>
@@ -16153,13 +16219,13 @@
     </row>
     <row r="106" spans="1:19" ht="21">
       <c r="A106" s="1" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="B106" s="8">
         <v>4</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="D106" t="s">
         <v>112</v>
@@ -16176,13 +16242,13 @@
     </row>
     <row r="107" spans="1:19" ht="21">
       <c r="A107" s="1" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B107" s="8">
-        <v>3</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>1056</v>
+        <v>1054</v>
+      </c>
+      <c r="B107" s="29">
+        <v>5</v>
+      </c>
+      <c r="C107" s="28" t="s">
+        <v>1147</v>
       </c>
       <c r="D107" t="s">
         <v>127</v>
@@ -16202,13 +16268,13 @@
     </row>
     <row r="108" spans="1:19" ht="21">
       <c r="A108" s="1" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="B108" s="8">
         <v>2</v>
       </c>
       <c r="C108" s="6" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="D108" t="s">
         <v>128</v>
@@ -16228,7 +16294,7 @@
     </row>
     <row r="109" spans="1:19" ht="21">
       <c r="A109" s="1" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="B109" s="8">
         <v>1</v>
@@ -16254,7 +16320,7 @@
     </row>
     <row r="110" spans="1:19" ht="21">
       <c r="A110" s="1" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="B110" s="8">
         <v>1</v>
@@ -16280,13 +16346,13 @@
     </row>
     <row r="111" spans="1:19" ht="105">
       <c r="A111" s="1" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="B111" s="8">
         <v>33</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="D111" t="s">
         <v>130</v>
@@ -16306,13 +16372,13 @@
     </row>
     <row r="112" spans="1:19" ht="21">
       <c r="A112" s="1" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="B112" s="8">
         <v>2</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="D112">
         <v>100</v>
@@ -16332,13 +16398,13 @@
     </row>
     <row r="113" spans="1:28" ht="21">
       <c r="A113" s="1" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="B113" s="8">
         <v>8</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="D113" t="s">
         <v>131</v>
@@ -16358,7 +16424,7 @@
     </row>
     <row r="114" spans="1:28" ht="21">
       <c r="A114" s="1" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="B114" s="8">
         <v>1</v>
@@ -16381,13 +16447,13 @@
     </row>
     <row r="115" spans="1:28" ht="42">
       <c r="A115" s="1" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="B115" s="8">
         <v>16</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="D115" t="s">
         <v>115</v>
@@ -16407,13 +16473,13 @@
     </row>
     <row r="116" spans="1:28" ht="21">
       <c r="A116" s="1" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="B116" s="8">
         <v>4</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D116" t="s">
         <v>133</v>
@@ -16433,13 +16499,13 @@
     </row>
     <row r="117" spans="1:28" ht="21">
       <c r="A117" s="1" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="B117" s="8">
         <v>5</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="D117" t="s">
         <v>134</v>
@@ -16456,7 +16522,7 @@
     </row>
     <row r="118" spans="1:28" ht="21">
       <c r="A118" s="1" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B118" s="8">
         <v>1</v>
@@ -16500,7 +16566,7 @@
     </row>
     <row r="119" spans="1:28" ht="21">
       <c r="A119" s="1" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B119" s="8">
         <v>1</v>
@@ -16523,13 +16589,13 @@
     </row>
     <row r="120" spans="1:28" ht="21">
       <c r="A120" s="1" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="B120" s="8">
         <v>2</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D120" t="s">
         <v>141</v>
@@ -16546,7 +16612,7 @@
     </row>
     <row r="121" spans="1:28" ht="21">
       <c r="A121" s="1" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="B121" s="8">
         <v>1</v>
@@ -16572,7 +16638,7 @@
     </row>
     <row r="122" spans="1:28" ht="21">
       <c r="A122" s="1" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="B122" s="8">
         <v>1</v>
@@ -16625,7 +16691,7 @@
     </row>
     <row r="123" spans="1:28" ht="21">
       <c r="A123" s="1" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="B123" s="8">
         <v>1</v>
@@ -16675,7 +16741,7 @@
     </row>
     <row r="124" spans="1:28" ht="21">
       <c r="A124" s="1" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="B124" s="8">
         <v>1</v>
@@ -16728,7 +16794,7 @@
     </row>
     <row r="125" spans="1:28" ht="21">
       <c r="A125" s="1" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="B125" s="8">
         <v>1</v>
@@ -16751,7 +16817,7 @@
     </row>
     <row r="126" spans="1:28" ht="21">
       <c r="A126" s="1" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="B126" s="8">
         <v>1</v>
@@ -16777,7 +16843,7 @@
     </row>
     <row r="127" spans="1:28" ht="21">
       <c r="A127" s="1" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="B127" s="8">
         <v>1</v>
@@ -16800,7 +16866,7 @@
     </row>
     <row r="128" spans="1:28" ht="21">
       <c r="A128" s="1" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="B128" s="8">
         <v>1</v>
@@ -16826,7 +16892,7 @@
     </row>
     <row r="129" spans="1:29" ht="21">
       <c r="A129" s="1" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="B129" s="8">
         <v>1</v>
@@ -16852,7 +16918,7 @@
     </row>
     <row r="130" spans="1:29" ht="21">
       <c r="A130" s="1" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="B130" s="8">
         <v>1</v>
@@ -16878,7 +16944,7 @@
     </row>
     <row r="131" spans="1:29" ht="21">
       <c r="A131" s="1" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="B131" s="8">
         <v>1</v>
@@ -16904,13 +16970,13 @@
     </row>
     <row r="132" spans="1:29" ht="21">
       <c r="A132" s="1" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="B132" s="8">
         <v>2</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="D132" t="s">
         <v>164</v>
@@ -16930,7 +16996,7 @@
     </row>
     <row r="133" spans="1:29" ht="21">
       <c r="A133" s="1" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="B133" s="8">
         <v>1</v>
@@ -16953,7 +17019,7 @@
     </row>
     <row r="134" spans="1:29" ht="21">
       <c r="A134" s="1" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="B134" s="8">
         <v>1</v>
@@ -16979,13 +17045,13 @@
     </row>
     <row r="135" spans="1:29" ht="21">
       <c r="A135" s="1" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="B135" s="8">
         <v>4</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="D135" t="s">
         <v>169</v>
@@ -17005,13 +17071,13 @@
     </row>
     <row r="136" spans="1:29" ht="21">
       <c r="A136" s="1" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="B136" s="8">
         <v>8</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="D136" t="s">
         <v>171</v>
@@ -17028,7 +17094,7 @@
     </row>
     <row r="137" spans="1:29" ht="21">
       <c r="A137" s="1" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="B137" s="8">
         <v>1</v>
@@ -17066,7 +17132,7 @@
     </row>
     <row r="138" spans="1:29" ht="21">
       <c r="A138" s="1" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="B138" s="8">
         <v>1</v>
@@ -17089,7 +17155,7 @@
     </row>
     <row r="139" spans="1:29" ht="21">
       <c r="A139" s="1" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="B139" s="8">
         <v>1</v>
@@ -17112,7 +17178,7 @@
     </row>
     <row r="140" spans="1:29" ht="21">
       <c r="A140" s="1" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="B140" s="8">
         <v>1</v>
@@ -17147,7 +17213,7 @@
   </sheetPr>
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
@@ -17164,7 +17230,7 @@
   <sheetData>
     <row r="1" spans="1:29">
       <c r="A1" s="14" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="12"/>
@@ -17246,10 +17312,10 @@
         <v>3</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>188</v>
@@ -17335,7 +17401,7 @@
         <v>13</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -17382,7 +17448,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
@@ -17429,7 +17495,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -17476,7 +17542,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -17523,7 +17589,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -17570,7 +17636,7 @@
         <v>67</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -17599,13 +17665,13 @@
     </row>
     <row r="10" spans="1:29" ht="63">
       <c r="A10" s="14" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="B10" s="20">
         <v>5</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>134</v>
@@ -17617,7 +17683,7 @@
         <v>135</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -17646,7 +17712,7 @@
     </row>
     <row r="11" spans="1:29" ht="21">
       <c r="A11" s="14" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="B11" s="20">
         <v>1</v>
@@ -17655,7 +17721,7 @@
         <v>795</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>796</v>
@@ -17664,7 +17730,7 @@
         <v>137</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -17705,7 +17771,7 @@
     </row>
     <row r="12" spans="1:29" ht="21">
       <c r="A12" s="14" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="B12" s="20">
         <v>1</v>
@@ -17723,7 +17789,7 @@
         <v>140</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -17752,13 +17818,13 @@
     </row>
     <row r="13" spans="1:29" ht="21">
       <c r="A13" s="14" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="B13" s="20">
         <v>2</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>141</v>
@@ -17770,7 +17836,7 @@
         <v>142</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -17799,7 +17865,7 @@
     </row>
     <row r="14" spans="1:29" ht="21">
       <c r="A14" s="14" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="B14" s="20">
         <v>1</v>
@@ -17817,7 +17883,7 @@
         <v>140</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
@@ -17864,7 +17930,7 @@
     </row>
     <row r="15" spans="1:29" ht="21">
       <c r="A15" s="14" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="B15" s="20">
         <v>1</v>
@@ -17873,7 +17939,7 @@
         <v>819</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>820</v>
@@ -17882,7 +17948,7 @@
         <v>147</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -17927,7 +17993,7 @@
     </row>
     <row r="16" spans="1:29" ht="21">
       <c r="A16" s="14" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="B16" s="20">
         <v>1</v>
@@ -17936,7 +18002,7 @@
         <v>826</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="E16" s="22" t="s">
         <v>827</v>
@@ -17945,7 +18011,7 @@
         <v>150</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -17992,7 +18058,7 @@
     </row>
     <row r="17" spans="1:29" ht="21">
       <c r="A17" s="14" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="B17" s="20">
         <v>1</v>
@@ -18010,7 +18076,7 @@
         <v>152</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
@@ -18039,7 +18105,7 @@
     </row>
     <row r="18" spans="1:29" ht="21">
       <c r="A18" s="14" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="B18" s="20">
         <v>1</v>
@@ -18057,7 +18123,7 @@
         <v>156</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
@@ -18104,7 +18170,7 @@
         <v>80</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="S19" t="s">
         <v>30</v>
@@ -18118,7 +18184,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>83</v>
@@ -18130,7 +18196,7 @@
         <v>84</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="S20" t="s">
         <v>30</v>
@@ -18156,7 +18222,7 @@
         <v>78</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="S21" t="s">
         <v>30</v>
@@ -18173,7 +18239,7 @@
         <v>208</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>209</v>
@@ -18182,7 +18248,7 @@
         <v>6</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="S22" t="s">
         <v>30</v>
@@ -18199,7 +18265,7 @@
         <v>510</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>511</v>
@@ -18208,7 +18274,7 @@
         <v>101</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="S23" t="s">
         <v>30</v>

</xml_diff>